<commit_message>
source sample type vocabularies
</commit_message>
<xml_diff>
--- a/vocabulary/CUAHSI-SampleTypeCV.xlsx
+++ b/vocabulary/CUAHSI-SampleTypeCV.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iSamples\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iSamples\metadata\vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4589E8A-5D85-4F4C-91EC-5DBE2129A5B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0B2E72-90EF-46BC-822E-1735B0B43FE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="375" windowWidth="25845" windowHeight="14325" xr2:uid="{5EF4A5A3-67FB-4182-B767-7D0382A35E8E}"/>
+    <workbookView minimized="1" xWindow="7320" yWindow="2025" windowWidth="22290" windowHeight="13275" xr2:uid="{5EF4A5A3-67FB-4182-B767-7D0382A35E8E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All types" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All types'!$B$1:$B$35</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
   <si>
     <t>Term</t>
   </si>
@@ -246,15 +249,9 @@
     <t>Vadose Water Weekly</t>
   </si>
   <si>
-    <t>Object type</t>
-  </si>
-  <si>
     <t>material</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>piece of Earth Material</t>
   </si>
   <si>
@@ -289,6 +286,54 @@
   </si>
   <si>
     <t>sample type</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>CUAHSI SampleTypeCV</t>
+  </si>
+  <si>
+    <t>N.A.</t>
+  </si>
+  <si>
+    <t>EarthMaterial</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>aqueous solution</t>
+  </si>
+  <si>
+    <t>container</t>
+  </si>
+  <si>
+    <t>Specimen type</t>
+  </si>
+  <si>
+    <t>solid object</t>
+  </si>
+  <si>
+    <t>solid material</t>
+  </si>
+  <si>
+    <t>granular material</t>
+  </si>
+  <si>
+    <t>this is a purpose</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>aggregation</t>
+  </si>
+  <si>
+    <t>is this for rocks (trawling bottom of water body), or netting stuffin the water column?</t>
+  </si>
+  <si>
+    <t>Mixed organic and inorganic fragments</t>
   </si>
 </sst>
 </file>
@@ -671,80 +716,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F365B018-C5CF-46EB-A35A-BEA2C8DC1474}">
-  <dimension ref="A1:F35"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="25.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="4" width="25.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>78</v>
+    <row r="1" spans="1:8" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>79</v>
+      <c r="H1" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>80</v>
+      <c r="F2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -752,13 +816,22 @@
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
@@ -766,13 +839,22 @@
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -780,13 +862,22 @@
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -794,13 +885,22 @@
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
@@ -808,13 +908,22 @@
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
@@ -822,35 +931,64 @@
       <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>81</v>
+      <c r="E9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>22</v>
@@ -858,13 +996,22 @@
       <c r="D12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>24</v>
@@ -872,72 +1019,124 @@
       <c r="D13" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="B14" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="B15" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="B16" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="B17" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>80</v>
+      <c r="F17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
@@ -946,46 +1145,69 @@
       <c r="D19" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>83</v>
+      <c r="E19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>82</v>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>83</v>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>44</v>
@@ -993,13 +1215,25 @@
       <c r="D23" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>46</v>
@@ -1007,13 +1241,22 @@
       <c r="D24" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>48</v>
@@ -1021,123 +1264,201 @@
       <c r="D25" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="B26" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="B27" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>83</v>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>80</v>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="B30" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>82</v>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>83</v>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="2"/>
+      <c r="E33" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="B34" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="B35" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B35" xr:uid="{07C64FB7-A996-4977-84FC-0CCC729EC590}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Sample type"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>